<commit_message>
charset changed to utf8
</commit_message>
<xml_diff>
--- a/Dataset/snippetshindi.xlsx
+++ b/Dataset/snippetshindi.xlsx
@@ -17,7 +17,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="412">
   <si>
-    <t>मैं उस पर फिदा हो गया। "जनता के अफीम का व्यंग्य नहीं है?" "आप धर्म के बारे में सोच रहे हैं," उन्होंने जवाब दिया। “सारकैम नैतिक रूप से बेरफ्ट का ज़ैनक्स है।</t>
+    <t>मैं उस पर फिदा हो गया। "जनता के अफीम का व्यंग्य नहीं है?" "आप धर्म के बारे में सोच रहे हैं," उन्होंने जवाब दिया। “सारकैम नैतिक रूप से बेरफ्ट का ज़ेनैक्स है।</t>
   </si>
   <si>
     <t>मैं, तुम हो</t>
@@ -29,7 +29,7 @@
     <t>अवुन रिया</t>
   </si>
   <si>
-    <t>समय क्या हुआ है? "" एक बजे। "मैंने लगभग कुछ सोडा थूक दिया। दोपहर में।" नहीं। सुबह में। उस लानत सूरज को तुम मूर्ख मत बनने दो। झूठ बोलता हैं।</t>
+    <t>क्या समय है? "" एक बजे। "मैंने लगभग कुछ सोडा थूक दिया।" दोपहर में। "नहीं। सुबह में। उस लानत सूरज को तुम मूर्ख मत बनने दो। झूठ बोलता हैं।</t>
   </si>
   <si>
     <t>मैं</t>
@@ -41,19 +41,19 @@
     <t>आप</t>
   </si>
   <si>
-    <t>मैं पहले से ही बेहोश हो गया था की तुलना में 'चीजों को बदतर कैसे किया जा सकता है' यह जानकर मुझे कोई बेहतर महसूस होता है? आपका मतलब है कि मैं और भी कम डूब सकता हूं? ओह खुशी!</t>
-  </si>
-  <si>
-    <t>जब आप पिशाच के कमरे में होते हैं तो आप क्या करते हैं और सबसे खतरनाक आपको बताता है कि आप बहुत ज्यादा जानते हैं? आप बोल्ट मैंने क्या किया? मैंने पाखंड किया।</t>
-  </si>
-  <si>
-    <t>"ओह नहीं, निक" जैमे ने सर्वोच्च असंबद्धता के स्वर में कहा, "आप कैसे कर सकते हैं? जब मेरी पीठ एक मोमेमेंट के लिए बदल गई थी। और मेरा भोजन बहुत स्वादिष्ट था।</t>
+    <t>मैं पहले से ही बेहोश हो गया था की तुलना में 'चीजों को कैसे बदतर किया जा सकता है' यह जानकर मुझे कोई बेहतर महसूस होता है? आपका मतलब है कि मैं और भी कम डूब सकता हूं? ओह खुशी!</t>
+  </si>
+  <si>
+    <t>जब आप पिशाचों के कमरे में होते हैं तो आप क्या करते हैं और सबसे खतरनाक आपको बताता है कि आप बहुत ज्यादा जानते हैं? आप बोल्ट मैंने क्या किया? मैंने पाखण्ड किया।</t>
+  </si>
+  <si>
+    <t>"अरे नहीं, निक" जैमे ने बेहद असम्मानजनक झटकों के स्वर में कहा, "आप कैसे कर सकते हैं? जब मेरी पीठ एक मोमे के लिए बदल गई थी। और मेरा भोजन बहुत स्वादिष्ट था।</t>
   </si>
   <si>
     <t>निक, तुम</t>
   </si>
   <si>
-    <t>मैं कैप्टन डक्कन हूं। मैं इस सुविधा का प्रभारी हूं। "" कप्तान डक्कन, "रयान ने दोहराया।" आपसे मिलना अच्छा है। मैंने सुना है ... अच्छा ... तुम्हारे बारे में कुछ नहीं ...</t>
+    <t>मैं कैप्टन डक्कन हूं। मैं इस सुविधा का प्रभारी हूं। "" कप्तान डक्कन, "रयान ने दोहराया।" आपसे मिलकर अच्छा लगा। मैंने सुना है ... अच्छा ... तुम्हारे बारे में कुछ नहीं ...</t>
   </si>
   <si>
     <t>कप्तान डक्कन</t>
@@ -65,7 +65,7 @@
     <t>नाटक</t>
   </si>
   <si>
-    <t>मैं धूप में चमगादड़ या चमचमाता भी नहीं हूं। सुंदर महिलाओं में वेश्यावृत्ति के चित्रण के रूप में हॉलीवुड के पिशाचों का चित्रण लगभग उतना ही सटीक है।</t>
+    <t>मैं धूप में चमगादड़ या चमचमाता नहीं हूँ। सुंदर महिलाओं में वेश्यावृत्ति के चित्रण के रूप में हॉलीवुड के पिशाच का चित्रण लगभग उतना ही सटीक है।</t>
   </si>
   <si>
     <t>हॉलीवुड की, सुंदर महिला</t>
@@ -77,13 +77,13 @@
     <t>समष्टिवाद</t>
   </si>
   <si>
-    <t>मैंने उसके संकेत दिए हैं! मैंने उसे बहुत सारे संकेत दिए हैं। वह मुझसे क्या चाहती है? उसे मेरे दस्ताने के साथ चेहरे पर थप्पड़, और उसे सुबह में पिस्तौल को चुनौती देने के लिए?</t>
+    <t>मैंने उसके संकेत दिए हैं! मैंने उसे बहुत सारे संकेत दिए हैं। वह मुझसे क्या चाहती है? उसे मेरे दस्ताने के साथ चेहरे पर थप्पड़, और उसे चुनौती देने के लिए सुबह में पिस्तौल?</t>
   </si>
   <si>
     <t>उसे वह</t>
   </si>
   <si>
-    <t>इससे कोई फर्क नहीं पड़ता कि ग्लास आधा भरा हुआ खाली है। बस इसे पी लो जबकि हर कोई इसके बारे में बहस कर रहा है और शुक्र है कि आपके पास इसमें कुछ के साथ एक गिलास था!</t>
+    <t>इससे कोई फर्क नहीं पड़ता कि ग्लास आधा भरा हुआ आधा है। बस इसे पीते हैं जबकि हर कोई इसके बारे में बहस कर रहा है और शुक्र है कि आपके पास इसमें कुछ के साथ एक गिलास था!</t>
   </si>
   <si>
     <t>मुझे यकीन है कि उसने सोचा था कि वह रोलर स्केट्स पर एक वेनिला वेफर के साथ लड़ाई कर रही थी, लेकिन बहुत कम लोगों को पता था कि वह एक मकड़ी के सैंडविच के साथ लड़ाई कर रही थी।</t>
@@ -92,28 +92,28 @@
     <t>वह</t>
   </si>
   <si>
-    <t>युवा, आजकल, कल्पना करते हैं कि पैसा ही सब कुछ है। हाँ, लॉर्ड हेनरी बड़बड़ाया, अपने कोट में बटन-छेद का निपटान किया; और जब वे बड़े हो जाते हैं तो उन्हें पता चल जाता है।</t>
+    <t>युवा, आजकल, कल्पना करते हैं कि पैसा ही सब कुछ है। हाँ, लॉर्ड हेनरी बड़बड़ाया, अपने कोट में बटन-छेद का निपटान किया; और जब वे बड़े हो जाते हैं तो वे इसे जानते हैं।</t>
   </si>
   <si>
     <t>युवा, वे</t>
   </si>
   <si>
-    <t>[एक टोपी के बारे में] आप इसे रख सकते हैं और कह सकते हैं, "अरे आप, बिना टोपी वाला व्यक्ति! मुझे आपके पास कुछ नहीं मिला है! मैंने इसे कैसे प्राप्त किया? संभवतः समाज के लिए अधिक मूल्य होने के कारण।</t>
+    <t>[एक टोपी के बारे में] आप इसे रख सकते हैं और कह सकते हैं, "अरे आप, बिना टोपी वाला व्यक्ति! मुझे आपके पास कुछ नहीं मिला है! मैंने इसे कैसे प्राप्त किया? संभवतः समाज के लिए अधिक मूल्य होने से।</t>
   </si>
   <si>
     <t>आप, एक टोपी के बिना व्यक्ति</t>
   </si>
   <si>
-    <t>क्योंकि किसी के दिल को चीरते हुए, पहली बार, शायद ऐसा लगता है कि किसी व्यक्ति को स्वाभाविक रूप से स्वीकार करना चाहिए, जैसे कि कोई सांता खंड नहीं है।</t>
+    <t>क्योंकि किसी के दिल को चीरते हुए, पहली बार, संभवतः ऐसा लगता है कि किसी व्यक्ति को स्वाभाविक रूप से स्वीकार करना चाहिए, जैसे कि कोई सांता खंड नहीं है।</t>
   </si>
   <si>
     <t>बाहर, सांता क्लॉज</t>
   </si>
   <si>
-    <t>अगर आप ऐसा करने जा रहे हैं, तो क्या आपको बिस्तर पर बैठने का इतना मन नहीं करेगा? ' हेड बोर्ड के पास एक व्यंग्यात्मक आवाज़ आई। 'शायद तुम फर्श पर लुढ़क सकते थे।</t>
-  </si>
-  <si>
-    <t>आपने बहुत सी चीजों को याद किया है। लेकिन ज्यादातर मुझे लगता है कि आपने छोड़ने के कई अवसर गंवाए हैं। मुझे दरवाजे पर आपकी सहायता करने दें ताकि आप इसे अगले एक को याद न करें।</t>
+    <t>अगर आप ऐसा करने जा रहे हैं, तो क्या आपको बिस्तर पर बैठने का इतना मन नहीं करेगा? ' हेड बोर्ड के पास एक व्यंग्यात्मक आवाज आई। 'शायद आप फर्श पर इधर-उधर लुढ़क सकते थे।</t>
+  </si>
+  <si>
+    <t>आपने बहुत सी चीजों को याद किया है। लेकिन ज्यादातर मुझे लगता है कि आपने छोड़ने के कई अवसर गंवाए हैं। मुझे दरवाजे पर आपकी सहायता करने दें ताकि आप इसे अगले याद न करें।</t>
   </si>
   <si>
     <t>आप, आप, आप</t>
@@ -122,7 +122,7 @@
     <t>मुझे पूरा यकीन है कि आप मेरी गेंदों को देख चुके हैं, "मैंने अपनी पैंट की खोज करने वाले व्यक्ति से कहा।" अब आप उन्हें गिनने जा रहे हैं? क्योंकि मैं तुम्हें मुसीबत से बचाऊंगा। वहाँ दो है।</t>
   </si>
   <si>
-    <t>आप उन्हें पसंद करते हैं, "मुझे एहसास हुआ। नूह की भौंहें सवाल उठाती हैं।" लोगों की तरह। "" जैसा कि ... फर्नीचर के विपरीत। "" वे मेरे हिस्से हैं। "" यह मेरी समझ है, हाँ।</t>
+    <t>आप उन्हें पसंद करते हैं, "मुझे एहसास हुआ। नूह की भौंहों ने सवाल उठाया।" लोगों की तरह। "" जैसा कि ... फर्नीचर के विपरीत। "" वे मेरे हिस्से हैं। "" यह मेरी समझ है, हाँ।</t>
   </si>
   <si>
     <t>मैं अपने</t>
@@ -140,16 +140,16 @@
     <t>मैं, बच्चा, तुम, जासूस, तुम, तुम्हारे</t>
   </si>
   <si>
-    <t>क्या होगा अगर, "इंस्पेक्टर फ्राई ने उसी मादक लहजे में कड़े लहजे में जवाब दिया," हम सभी डेज़ी श्रृंखला का निर्माण करने और उन्हें देखने के लिए थे ताकि जनता के विचारों को ढाल सकें?</t>
+    <t>क्या होगा अगर, "इंस्पेक्टर फ्राई ने उसी मदहोश कर देने वाले लहजे में जवाब दिया," हम सब डेज़ी श्रृंखला का निर्माण कर रहे थे और उन्हें ढंक रहे थे ताकि जनता के नज़रिए से शब्दों को ढाल सकें?</t>
   </si>
   <si>
     <t>सार्वजनिक दृश्य से शब्दों को ढालने के लिए, बाहर</t>
   </si>
   <si>
-    <t>... जैसा कि उसकी आवाज़ में कटाक्ष हो सकता है। "हाँ, वह ऊपर से ब्लू ब्लीडिंग कर रहा है, लेकिन मुझे लगा कि मैं आपको तुरंत बताने से बचूंगा, क्योंकि मुझे सस्पेंस निकालना है।</t>
-  </si>
-  <si>
-    <t>जूल्स खड़े हो गए और गंभीर रूप से खिंच गए। "चलो जल्दी करो और भुगतान करने से पहले" उसने अपने अंगूठे की एक झिलमिलाहट के साथ क्लेयर को संकेत दिया- "कुछ चमकदार दिखता है और हम फिर से हार जाते हैं।</t>
+    <t>... जैसा कि उसकी आवाज़ में कटाक्ष था। "हाँ, वह ऊपर की ओर ब्ल्यू ब्लीडिंग कर रहा है, लेकिन मुझे लगा कि मैं आपको तुरंत बताने से बचूंगा, क्योंकि मुझे सस्पेंस निकालना है।</t>
+  </si>
+  <si>
+    <t>जूल्स खड़े हो गए और गंभीर रूप से खिंच गए। "चलो जल्दी करो और पहले वह भुगतान करें" -उसने अपने अंगूठे की झिलमिलाहट के साथ क्लेयर को संकेत दिया- "कुछ चमकदार दिखता है और हम फिर से हार जाते हैं।</t>
   </si>
   <si>
     <t>क्लेयर, उसकी</t>
@@ -161,7 +161,7 @@
     <t>कथा, प्रेमालाप, विवाह</t>
   </si>
   <si>
-    <t>बेटे, मेरे पिताजी ने कहा, हर आदमी को अपने जीवन में एक कड़वी, नाराज महिला की जरूरत होती है। क्योंकि एक माँ के दिल को छूने के अलावा और कुछ भी नहीं पता है कि उसका बेटा उसके बारे में लगातार सोचता है।</t>
+    <t>बेटे, मेरे पिताजी ने कहा, हर आदमी को अपने जीवन में एक कड़वी, नाराज महिला की जरूरत होती है। क्योंकि एक माँ के दिल को छूने के अलावा और कुछ भी नहीं है जिससे पता चले कि उसका बेटा उसके बारे में लगातार सोचता है।</t>
   </si>
   <si>
     <t>कड़वी, नाराज महिला</t>
@@ -170,10 +170,10 @@
     <t>अच्छा, बच्चा? क्या आप मुझे किसी प्रकार के अकथ्य जीव में बदलने की कोशिश नहीं कर रहे हैं? मुझे नहीं लगता कि मैं परेशान होऊंगा, मैडम, यह देखकर कि आप इसे खुद का इतना अच्छा काम बना रहे हैं!</t>
   </si>
   <si>
-    <t>मैं, मैडम, आप, आप, जैसा कि आप देख रहे हैं कि यह इतना अच्छा काम कर रही है</t>
-  </si>
-  <si>
-    <t>मुझे नहीं पता कि कारों पर "जादू होता है" के बारे में क्या है, लेकिन हर बार जब मैं देखता हूं कि मैं अपने स्थायी मार्कर को बाहर निकालना चाहता हूं और उसके नीचे चुपके से लिखता हूं "तो यह मृत्यु को दर्शाता है"।</t>
+    <t>मैं, मैडम, आप, आप, जैसा कि आप देख रहे हैं, यह एक अच्छा काम है</t>
+  </si>
+  <si>
+    <t>मुझे नहीं पता है कि कारों पर "जादू होता है" के बारे में क्या है, लेकिन हर बार जब मैं देखता हूं कि मैं अपने स्थायी मार्कर को बाहर निकालता हूं और उसके नीचे चुपके से लिखता हूं "तो यह मृत्यु को दर्शाता है"।</t>
   </si>
   <si>
     <t>जादू होता है स्टिकर</t>
@@ -182,7 +182,7 @@
     <t>मेरे पास रविवार को चर्च है। "" बेशक आप करते हैं। "" आपका साथ आने का स्वागत है। "" धन्यवाद, लेकिन मैं धूप लगाना चाहता हूं। "" यह शर्म की बात है। "" यह मेरे अस्तित्व का प्रतिबंध है। ”- बेथ और जेक</t>
   </si>
   <si>
-    <t>ओह, भगवान के प्यार के लिए। आपसे ज्यादा कोई एजेंट नहीं है। मैं कसम खाता हूँ कि आपके डीएनए में एन्क्रिप्टेड पिन-धारीदार संबंध हैं। जब आप मर जाते हैं, तो ताबूत एफबीआई की संपत्ति पढ़ने वाला है।</t>
+    <t>ओह, भगवान के प्यार के लिए। आपसे ज्यादा कोई एजेंट नहीं है। मुझे लगता है कि आपके पास आपके डीएनए में पिन-स्ट्रिप किए गए संबंध हैं। जब आप मर जाते हैं, तो ताबूत एफबीआई की संपत्ति को पढ़ने जा रहा है।</t>
   </si>
   <si>
     <t>आप अपने</t>
@@ -194,22 +194,22 @@
     <t>टेस, कैफीन, यह स्थिति</t>
   </si>
   <si>
-    <t>सिल्वरस्ट्रीम: यू इडियट !!! तुम मेरे क्षेत्र में क्या कर रहे हो ??? ग्रेस्ट्रिप: ... डूबना? सिल्वरस्ट्रीम: क्या आप ऐसा अपने क्षेत्र में नहीं कर सकते? ग्रेस्ट्रिप: आह, लेकिन मुझे वहाँ कौन बचाएगा?</t>
+    <t>सिल्वरस्ट्रीम: यू इडियट !!! तुम मेरे क्षेत्र में क्या कर रहे हो ??? ग्रेस्ट्रिप: ... डूबना? सिल्वरस्ट्रीम: क्या आप ऐसा अपने क्षेत्र में नहीं कर सकते? ग्रेस्ट्रिप: आह, लेकिन मुझे वहां कौन बचाएगा?</t>
   </si>
   <si>
     <t>सिल्वरस्ट्रीम</t>
   </si>
   <si>
-    <t>हमारे पास और घटना थी। मैंने इसका ध्यान रखा। "" रियली। "जेसीस की आवाज ने कटाक्ष किया।" क्या आप भी जानते हैं कि चाकू, क्लेरिसा का उपयोग कैसे किया जाता है। अपने आप को या किसी निर्दोष समझने वाले को छेद दिए बिना?</t>
+    <t>हमारे पास और घटना थी। मैंने इसका ध्यान रखा। "" रियली। "जेक की आवाज ने कटाक्ष किया।" क्या आप भी जानते हैं कि उस चाकू, क्लेरिसा का उपयोग कैसे किया जाता है? अपने आप को या किसी निर्दोष समझने वालों को छेद दिए बिना?</t>
   </si>
   <si>
     <t>मैं, क्लेरिसा, आप, स्वयं</t>
   </si>
   <si>
-    <t>सुनो, पीचिस, प्रवंचना है कि मनुष्य क्या कर रहे हैं, "मौरिस की आवाज ने कहा।" वे हर समय एक दूसरे को धोखा देने के लिए उत्सुक हैं कि वे सरकारों को उनके लिए ऐसा करने के लिए चुनते हैं।</t>
-  </si>
-  <si>
-    <t>मनुष्य, वे, वे, एक-दूसरे को हर समय बरगलाते रहते हैं, वे, वे, सरकारें, यह</t>
+    <t>सुनो, पीचिस, प्रवंचना है जो मनुष्य के बारे में हैं, "मौरिस की आवाज ने कहा।" वे हर समय एक दूसरे को धोखा देने के लिए इतने उत्सुक हैं कि वे सरकारों को उनके लिए ऐसा करने के लिए चुनते हैं।</t>
+  </si>
+  <si>
+    <t>मनुष्य, वे, वे, हर समय एक दूसरे को धोखा देते हैं, वे, उन्हें, सरकारें, यह</t>
   </si>
   <si>
     <t>प्यार को चारा के रूप में उपयोग करना और अहंकार-लाड़ के साथ सम्मान की जगह लेना आपको एक कुशल सामाजिक जानवर बनाता है; दुर्भाग्य से, सभी प्रकार के जानवर मनुष्य की तुलना में कम विकसित हैं। क्या आप विकसित करना चाहेंगे?</t>
@@ -218,7 +218,7 @@
     <t>प्रेम को चारा की तरह इस्तेमाल करते हुए, अहंकार-लाड़ से सम्मान की जगह, आप</t>
   </si>
   <si>
-    <t>ये हुई ना बात! इसे चिकन शोरबा बनाएं या कुछ भी नहीं। वह पुराना पैर नीचे रख रहा है। यदि वह एक नर्वस ब्रेकडाउन का निर्धारण करती है, तो कम से कम हम यह देख सकते हैं कि उसके पास शांति नहीं है।</t>
+    <t>ये हुई ना बात! इसे चिकन शोरबा बनाएं या कुछ भी नहीं। वह पुराना पैर नीचे रख रहा है। अगर वह नर्वस ब्रेकडाउन होने के लिए दृढ़ है, तो कम से कम हम यह देख सकते हैं कि उसके पास यह शांति नहीं है।</t>
   </si>
   <si>
     <t>पुजारी वैसे भी सिर में थोड़ा अजीब हैं, "पुजारी ने निंदनीय रूप से जोड़ा," यही वजह है कि चर्च ने उन्हें मानसिक अस्पतालों में बंद कर दिया और व्यर्थ ही इन संस्थानों को मठ कहते हैं।</t>
@@ -233,7 +233,7 @@
     <t>उसके पिता, पिताजी</t>
   </si>
   <si>
-    <t>हो सकता है, "उन्होंने धीमे, ग्रामीण आह्वान में कहा," आप मुझे समझा सकते हैं कि मैंने आपको एक तांडव के बीच में क्यों पाया। "" ठीक है, "मैंने कहा," अगर आप एक तांडव में रहने जा रहे हैं, तो " मध्य सबसे अच्छा स्थान है, यह नहीं है।</t>
+    <t>हो सकता है, "उन्होंने धीमे, ग्रामीण आह्वान में कहा," आप मुझे समझा सकते हैं कि मैंने आपको एक तांडव के बीच में क्यों पाया। "" ठीक है, "मैंने कहा," अगर आप एक तांडव में रहने जा रहे हैं, तो " मध्य सबसे अच्छा स्थान है, है ना।</t>
   </si>
   <si>
     <t>वह, मैं, नंगा नाच, यह</t>
@@ -251,16 +251,16 @@
     <t>कप्तान आत्महत्या, आप, मैं, आप, आप, वह</t>
   </si>
   <si>
-    <t>तेईस कहानियाँ ऊपर और सभी मैं देख सकता था कि खिड़कियां ग्रे स्मॉग थीं। वे चाहते तो एंजल्स का शहर कह सकते थे, लेकिन अगर वहाँ से फ़रिश्ते निकलते तो उन्हें अंधाधुंध उड़ना पड़ता।</t>
+    <t>तेईस कहानियाँ ऊपर और सब मैं देख सकता था कि खिड़कियां धूसर धुँधली थीं। वे चाहते तो एंजल्स का शहर कह सकते थे, लेकिन अगर वहाँ से फ़रिश्ते निकलते तो उन्हें अंधाधुंध उड़ना पड़ता।</t>
   </si>
   <si>
     <t>यह, वे, वे, एन्जिल्स के शहर</t>
   </si>
   <si>
-    <t>आपने जो किया है, उसे देखिए, ’’ संगीन ने अपने सिर को नकली गंभीरता से हिलाते हुए कहा। 'तुमने कपटपूर्ण छोटी साजिश को नाकाम कर दिया है। आप विजयी और विजयी हुए हैं। तुम्हें शाप देते हैं, करो-भला करो। तुम्हें श्राप लगे।</t>
-  </si>
-  <si>
-    <t>मुझे अक्सर उल्लेखनीय रूप से उज्ज्वल होने के बारे में सोचा जाता है, और फिर भी मेरे दिमाग, अधिक से अधिक बार नहीं, मेरे दुश्मनों को अचानक, गैगिंग, लेखन, मौत की ओर अग्रसर करने के नए और दिलचस्प तरीके विकसित कर रहे हैं।</t>
+    <t>आपने जो किया है, उसे देखिए, ’’ संगीन ने अपने सिर को नकली गंभीरता से हिलाते हुए कहा। 'तुमने कपटपूर्ण छोटी साजिश को नाकाम कर दिया है। आप विजयी और विजयी हुए हैं। लानत है तुम्हें, कुकर्म करने वालों की। तुम्हें श्राप लगे।</t>
+  </si>
+  <si>
+    <t>मुझे अक्सर उल्लेखनीय रूप से उज्ज्वल होने के बारे में सोचा जाता है, और फिर भी मेरे दिमाग, अधिक से अधिक बार नहीं, मेरे दुश्मनों को अचानक, गैगिंग, writhing, agonizing मौत लाने के नए और दिलचस्प तरीके से व्यस्त कर रहे हैं।</t>
   </si>
   <si>
     <t>मैं, मेरा, मेरा दिमाग</t>
@@ -272,7 +272,7 @@
     <t>श्री मार्शल</t>
   </si>
   <si>
-    <t>अपने हथियारों को सुरक्षित रूप से संग्रहीत करने का सबसे अच्छा स्थान आपके दुश्मन के हाथों में है। यह आपके हित में है कि आप बेफिक्र रहें जबकि आपके शासकों के पास सभी हथियार हैं। आखिरकार, सरकार जानती है कि आपके लिए सबसे अच्छा क्या है।</t>
+    <t>अपने हथियारों को सुरक्षित रूप से संग्रहीत करने का सबसे अच्छा स्थान आपके दुश्मन के हाथों में है। यह आपके हित में है कि आप बेफिक्र रहें जबकि आपके शासकों के पास सभी हथियार हैं। आखिरकार, सरकार को पता है कि आपके लिए सबसे अच्छा क्या है।</t>
   </si>
   <si>
     <t>तुम्हारे तुम</t>
@@ -284,10 +284,10 @@
     <t>ओह, आपको निक को धोखा देने के लिए एलन की आवश्यकता है और फिर आप निक की शक्तियों को चुरा लेंगे और उन दोनों को मार देंगे, "मॅई ने कहा।" महान विचार। अरे, क्या मैं आ सकता हूं? यदि आप सैंडविच पर खून नहीं आने देने का वादा करते हैं तो मैं एक पिकनिक लंच लाऊंगा।</t>
   </si>
   <si>
-    <t>विचार, आप, आप</t>
-  </si>
-  <si>
-    <t>वह केवल लग रहा था ... नाराज। कष्टप्रद, और पसीने से तर, और गर्म। "हाँ, ठीक है," उन्होंने कहा, "अगली बार जब आप हमारे जादुई वार्ड वाले अपार्टमेंट से एक दरवाज़े से बाहर निकलने का फैसला करते हैं जो वास्तव में मौजूद नहीं होना चाहिए, तो एक नोट छोड़ दें।</t>
+    <t>विचार, आप, आप करेंगे</t>
+  </si>
+  <si>
+    <t>वह केवल लग रहा था ... नाराज। कष्टप्रद, और पसीने से तर, और गर्म। "हाँ, ठीक है," उन्होंने कहा, "अगली बार जब आप एक जादुई दरवाजे से हमारे जादुई अपार्टमेंट से बाहर निकलने का फैसला करते हैं जो वास्तव में मौजूद नहीं होना चाहिए, तो एक नोट छोड़ दें।</t>
   </si>
   <si>
     <t>आप, अपार्टमेंट</t>
@@ -299,37 +299,37 @@
     <t>मेरा मे</t>
   </si>
   <si>
-    <t>... जबकि डैनियल अपने कमरे में गायब हो गया, शायद अपने इंटर्नशिप अनुप्रयोगों के लिए दार्शनिक बकवास के कुछ अति सुंदर नक्षत्रों की आकृति को सीमित करने और अपने अति उत्साही ओसीडी के गले में हांफते हुए।</t>
+    <t>... जबकि डैनियल अपने कमरे में गायब हो गया, शायद अपने इंटर्नशिप अनुप्रयोगों के लिए दार्शनिक बकवास के कुछ अति सुंदर नक्षत्रों के आकृति को सीमित करने और अपने अति उत्साही ओसीडीस के गले में हांफते हुए।</t>
   </si>
   <si>
     <t>डैनियल, उसकी</t>
   </si>
   <si>
-    <t>तुम मुझे क्षमा करोगे, "उसने आखिर कहा," अगर यह सुझाव कि माइनसक्यूल ब्लैक शलजम आप एक दिल कहते हैं, अचानक मेरे साथ उदारता के साथ बह निकला है जो मुझे खुद को छोड़ना चाहता है और एक दीवार के खिलाफ मेरी पीठ थपथपाता है।</t>
+    <t>तुम मुझे क्षमा करोगे, "उसने आखिर कहा," अगर यह सुझाव कि माइनसक्यूल ब्लैक शलजम आप एक दिल कहते हैं, अचानक मेरे साथ उदारता के साथ बह निकला है, जो मुझे अपने आप को छोड़ना चाहता है और एक दीवार के खिलाफ मेरी पीठ थपथपाता है।</t>
   </si>
   <si>
     <t>तुम, सुझाव, तुम, miniscule काले शलजम होगा</t>
   </si>
   <si>
-    <t>क्या आप शीज़ पर कुछ भी सीखने की उम्मीद करते हैं? "उन्होंने पूछा। मैंने पहले ही सीखा है कि अजनबियों से बात नहीं करना चाहिए।" "फिर मैं अपना परिचय दूंगा और हम अजनबी नहीं रह जाएंगे। मैं डिलमोंड हूं। "" मैं तुम्हें जानने के लिए निर्वस्त्र हूं।</t>
+    <t>क्या आप शीज़ पर कुछ भी सीखने की उम्मीद करते हैं? "उन्होंने पूछा।" मैंने पहले ही अजनबियों से बात नहीं करना सीख लिया है। "" तब मैं अपना परिचय दूंगा और हम अजनबी नहीं रह जाएंगे। मैं डिलमोंड हूं। "" मैं तुम्हें जानने के लिए निर्वस्त्र हूं।</t>
   </si>
   <si>
     <t>मैं, डिलमोंड, आप</t>
   </si>
   <si>
-    <t>आप एक अच्छी तरह से सम्मानित एजेंट, माइकल, एक लत्ता-से-समृद्ध धन कथा समाप्त हो रहे थे। जब तक आप बदनाम नहीं हो जाते। अब यह प्रतीत होता है कि आपका अपना संगठन आपसे छुटकारा चाहता है। यह क्यों है? "" मेरी बंदूक वापस एक कद्दू में बदल गई।</t>
+    <t>आप एक अच्छी तरह से सम्मानित एजेंट, माइकल, एक लत्ता-से-समृद्ध धन कहानी समाप्त हो रहे थे। जब तक आप बदनाम नहीं हो जाते। अब यह प्रतीत होता है कि आपका अपना संगठन आपसे छुटकारा चाहता है। यह क्यों है? "" मेरी बंदूक वापस एक कद्दू में बदल गई।</t>
   </si>
   <si>
     <t>बाहर</t>
   </si>
   <si>
-    <t>गोटे ने मेरा मेक अप किया है, अगर मैं जॉय में दौड़ता हूं और वह मुझसे बाहर निकलना चाहता है। मेरी सबसे अच्छी लग रही होगी! शायद वह मुझे बार-बार किडनी और पेट में घूंसे मारेगा, ताकि मेरे चेहरे पर निशान न पड़े। वह बहुत विचारशील है!</t>
+    <t>गोटे ने मेरा मेक अप किया है, अगर मैं जॉय में दौड़ता हूं और वह मुझसे बाहर निकलना चाहता है। होगा मेरा सबसे अच्छा देखो! हो सकता है कि वह मुझे बार-बार किडनी और पेट में घूंसे मारे, ताकि मेरे चेहरे पर निशान न पड़े। वह बहुत विचारशील है!</t>
   </si>
   <si>
     <t>जॉय, वह, वह, वह हूँ</t>
   </si>
   <si>
-    <t>आपने जिन लोगों के बारे में पढ़ा है, उनमें से अधिकांश क्लबों या इंटरनेट पर वैम्प्स से मिलते-जुलते हैं ... ईव, क्या आपने ...? "" हाँ, मैं इंटरनेट पर एक पिशाच से मिला, उसकी बुराई से प्यार किया, और उसे जाने दिया मुझे घुमाओ, क्योंकि मैं वह बुद्धिहीन हूँ।</t>
+    <t>आपने जिन लोगों के बारे में पढ़ा है, उनमें से अधिकांश क्लबों या इंटरनेट पर वैम्प्स से मिलते-जुलते हैं ... ईव, क्या आपने ...? "" हाँ, मैं इंटरनेट पर एक पिशाच से मिला, उसकी बुराई से प्यार हुआ, और उसे जाने दिया मुझे घुमाओ, क्योंकि मैं वह बुद्धिहीन हूं।</t>
   </si>
   <si>
     <t>गुरुवार की दोपहर है, और हमारे पास खेल हैं। ये लड़कियों के लिए विकल्प हैं: एक आमंत्रण क्रिकेट खेल देखना; कक्षाओं में से एक में अध्ययन; या सीनियर रग्बी लीग देख रहे हैं। जैसा कि आप कल्पना कर सकते हैं, मैं फटा हुआ हूँ।</t>
@@ -338,13 +338,13 @@
     <t>लड़कियों के लिए विकल्प, विकल्प, एक आमंत्रण क्रिकेट खेल देखना, कक्षाओं में से एक में अध्ययन करना, सीनियर रग्बी लीग देखना</t>
   </si>
   <si>
-    <t>वह मेरी सबसे अच्छी दोस्त है, और मुझे पता है कि उसका मतलब अच्छी तरह से है, लेकिन जैसा कि वह बात करती है मैं मानसिक रूप से उन सभी तरीकों की गणना कर रही हूं, जो मैं उसे चुप करा सकती थी। मैं उससे बड़ा हूं ... मुझे आश्चर्य है कि अगर मैं अपने स्ट्रगल को किसी प्रकार के मैकगाइवर से प्रेरित हथियार के लिए इस्तेमाल कर सकता हूं।</t>
+    <t>वह मेरी सबसे अच्छी दोस्त है, और मुझे पता है कि उसका मतलब अच्छी तरह से है, लेकिन जैसा कि वह बात करती है मैं मानसिक रूप से उन सभी तरीकों की गणना कर रहा हूं जो मैं उसे चुप करा सकता था। मैं उससे बड़ा हूं ... मुझे आश्चर्य है कि अगर मैं अपने स्ट्रगल को किसी प्रकार के मैकगाइवर से प्रेरित हथियार के लिए इस्तेमाल कर सकता हूं।</t>
   </si>
   <si>
     <t>वह, वह, उसका है</t>
   </si>
   <si>
-    <t>मैं अपने गालों में उठती गर्मी को महसूस कर सकता था। 'हमने एक रात एक साथ बिताई।' 'आपने तब सेक्स किया था?' 'नहीं, हम एक रजाई crocheted।' मैंने अपने सिर को साइड में कर दिया और उसे अपनी सबसे गहरी चकाचौंध दे दी। "लोरेली प्रेस्टन टू एजेंट ब्रॉडी-द हंट हंट</t>
+    <t>मैं अपने गालों में उठती गर्मी को महसूस कर सकता था। 'हमने एक रात एक साथ बिताई।' 'आपने तब सेक्स किया था?' 'नहीं, हम एक रजाई crocheted।' मैंने अपने सिर को साइड में कर दिया और उसे मेरी नातिन की चकाचौंध दी। "लोरेले प्रेस्टन को एजेंट ब्रूडी-द हंट</t>
   </si>
   <si>
     <t>उसे, एजेंट ब्रॉडी</t>
@@ -356,16 +356,16 @@
     <t>यह, उसका जीवन, वह, वह, उसका यह जीवन, उसका, वह</t>
   </si>
   <si>
-    <t>क्या आप हाउस-वाइफ, मिसेज सिल्वर हैं? ' उसने पूछा। 'सफेद शर्ट से बर्गर रीलीज़ करवाने के लिए आप क्या सलाह देंगे?' सीलिंग करने वाली महिला ने ग्यारह तक अपने टकटकी के विष-स्तर को क्रैंक किया, और रेवेन सुखद ढंग से मुस्कुराया।</t>
+    <t>क्या आप एक हाउस-वाइफ, मिसेज सिल्वर हैं? ' उसने पूछा। 'सफेद शर्ट से बर्गर रीलीज़ करवाने के लिए आप क्या सलाह देंगे?' सीलिंग करने वाली महिला ने ग्यारह तक अपने टकटकी के विष-स्तर को क्रैंक किया, और रेवेन सुखद ढंग से मुस्कुराया।</t>
   </si>
   <si>
     <t>आप, हाउस-वाइफ, मिसेज सिल्वर, सिल्वर, द सेमिटिंग वुमन, विमेन, उसकी</t>
   </si>
   <si>
-    <t>मैं आप लोगों से नहीं मिलता। आप टेलीविज़न पर गॉडफादर देखते हैं और टन के लोग गोली मारकर हत्या कर रहे हैं, हर जगह खून बिखरा हुआ है और यह मनोरंजक है। लेकिन, जब उन्होंने एक घोड़े को मार दिया, तो लोग नाराज हो गए।</t>
-  </si>
-  <si>
-    <t>आप लोग, आप, आप, यह, उन्होंने एक घोड़े को मार डाला, लोगों को</t>
+    <t>मैं आप लोगों से नहीं मिलता। आप टेलीविज़न पर गॉडफादर देखते हैं और लोगों को गोली मार दी जाती है और चाकू मार दिया जाता है, हर जगह खून बिखरा हुआ है और यह मनोरंजक है। लेकिन, जब उन्होंने एक घोड़े को मार दिया, तो लोग नाराज हो गए।</t>
+  </si>
+  <si>
+    <t>आप लोग, आप, आप, यह, उन्होंने एक घोड़ा, लोगों को मार डाला</t>
   </si>
   <si>
     <t>सोशल मीडिया ने हम सभी को कुत्तों में बदल दिया है। जिस समय एक अकेला कुत्ता किसी चीज़ से दुखी होता है, वह भौंकने लगता है और फिर सैकड़ों अन्य लोग भौंकने में तुरंत शामिल हो जाते हैं। हम अब अपने दिमाग का उपयोग नहीं करते हैं, हम सिर्फ कोरस में शामिल होते हैं।</t>
@@ -380,13 +380,13 @@
     <t>विस्फोटक पैकेज, हम, हम</t>
   </si>
   <si>
-    <t>अगर केवल इस छोटे कार्ड पर पर्याप्त जगह थी तो आपने जो किया है उसके लिए मेरे अनफिट जोए डे विवर को निकालने के लिए। उल्लास, मिर्थ, हर पुतला सेल की स्वर्गीय बुदबुदाती है जो मेरे अंदर आपकी दया और पिटाई के लिए गाती है।</t>
+    <t>अगर केवल इस छोटे कार्ड पर पर्याप्त जगह थी तो आपने जो किया है उसके लिए मेरे अनफिट जोए डे विवर को निकालने के लिए। उल्लास, मिर्थ, हर पुतला सेल की स्वर्गीय बुदबुदाती है जो मेरे अंदर आपकी दया और पिटाई की भेंट चढ़ती है।</t>
   </si>
   <si>
     <t>आप, आपकी दयालु और पवित्र भेंट, आपका, यह छोटा कार्ड, कार्ड</t>
   </si>
   <si>
-    <t>अजीब बात है कि यह है, सरोव अभी भी तुम्हारे बारे में परवाह है। उसने मुझसे कहा कि तुमको अकेला छोड़ दूं। लेकिन मुझे लगता है, इस बार, मुझे जनरल की अवज्ञा करनी चाहिए। तुम मेरे हो! और मेरा इरादा आपको पीड़ित बनाने का है ... "" आपसे बात करने से मुझे तकलीफ होती है, "एलेक्स ने कहा।</t>
+    <t>अजीब बात है कि यह है, सरोव अभी भी तुम्हारे बारे में परवाह है। उसने मुझसे कहा कि तुमको अकेला छोड़ दूं। लेकिन मुझे लगता है, इस बार, मुझे जनरल की अवज्ञा करनी चाहिए। तुम मेरे हो! और मेरा इरादा आपको पीड़ित बनाने का है ... "" सिर्फ आपसे बात करने से मुझे तकलीफ होती है, "एलेक्स ने कहा।</t>
   </si>
   <si>
     <t>आप से बात कर रहा हूँ</t>
@@ -398,31 +398,31 @@
     <t>सरकार और जनता, सरकार, जनता, उनका, उनका, उन्होंने</t>
   </si>
   <si>
-    <t>फिर तुम यहाँ क्यों हो? "एम्मा ने माँग की।" ओह, क्या यह उन मिस-कनेक्शन चीजों में से एक है? हम दूसरी रात मिले, आपको एक चिंगारी लगी? क्षमा करें, लेकिन मैं पेड़ नहीं लगाता। "" मैं पेड़ नहीं हूं। "इरलथ गुस्से में दिखे, उनकी छाल थोड़ी छील गई।</t>
-  </si>
-  <si>
-    <t>तुम, उन कनेक्शन चीजों को याद किया, तुम एक चिंगारी लगा</t>
-  </si>
-  <si>
-    <t>मिस प्रेंड्रैजैस्ट! "उन्होंने अपने पोर पर अपने घुटनों के बल बैठकर रेप किया।" आप कभी किसी खतरे में नहीं थे! "" जंगली जानवरों को छोड़कर। "उसकी पलकें झपक गई मानो उसे देख कर एक रेप्रीव की जरूरत हो।" खरगोश द्वारा हमला किया गया।</t>
-  </si>
-  <si>
-    <t>मिस प्रेंड्रैजैस्ट, प्रेंड्रैजैस्ट, यू, उसकी, आप, खरगोश, खरगोश ने हमला किया</t>
-  </si>
-  <si>
-    <t>ओह, अपने आप को समायोजित करें। आप लोगों ने कभी अधिक समर्पित नागरिक बनने के दौरान सैनिकों पर दस सहस्राब्दी खेलने में खर्च किया है। हमने पिछले हज़ार साल बिताए हैं कि जीती हुई गांगेय युद्ध की विरासत को परिष्कृत करते हुए नागरिक बने रहने की कोशिश कर रहे हैं।</t>
+    <t>फिर तुम यहाँ क्यों हो? "एम्मा ने माँग की।" ओह, क्या यह उन मिस-कनेक्शन चीजों में से एक है? हम दूसरी रात मिले, आपको एक चिंगारी लगी? क्षमा करें, लेकिन मैं पेड़ नहीं लगाता। "" मैं एक पेड़ नहीं हूं। "इरलथ गुस्से में दिखे, उनकी छाल थोड़ी छील गई।</t>
+  </si>
+  <si>
+    <t>तुम, उन चीजों को याद किया, तुम एक चिंगारी लगा</t>
+  </si>
+  <si>
+    <t>मिस प्रेंड्रेगैस्ट! "उन्होंने अपने पोर पर अपनी अंगुलियों के बल पर रेप किया।" आप कभी किसी खतरे में नहीं थे! "" जंगली जानवरों को छोड़कर। "उसकी पलकें झपक गई जैसे कि उसे देखने से किसी दुःख की आवश्यकता हो।" खरगोश द्वारा हमला किया गया।</t>
+  </si>
+  <si>
+    <t>मिस प्रेंड्रैजैस्ट, प्रेंड्रैगैस्ट, यू, उसकी, आप, खरगोश, खरगोश ने हमला किया</t>
+  </si>
+  <si>
+    <t>ओह, अपने आप को समायोजित करें। आप लोगों ने कभी अधिक समर्पित नागरिक बनने के दौरान सैनिकों पर खेलने के लिए दस सहस्राब्दी खर्च किए हैं। हमने पिछले हज़ार साल बिताए हैं कि जीती हुई गांगेय युद्ध की विरासत को परिष्कृत करते हुए नागरिक बने रहने की कोशिश कर रहे हैं।</t>
   </si>
   <si>
     <t>आप, आप लोग, आप</t>
   </si>
   <si>
-    <t>मुझे इसमें कोई संदेह नहीं है कि जब मेरी पीठ मुड़ी होगी तो वे आपको मेरे बारे में कई तरह की बातें बताएंगे। हो सकता है कि वे उस समय पीछे नहीं रहे जब भगवान ने सुंदर चेहरों को पास किया, लेकिन स्वर्ग केवल जानता है कि वे कहाँ थे जब उन्होंने कृतज्ञता को विभाजित किया था।</t>
+    <t>मुझे इसमें कोई संदेह नहीं है कि जब मेरी पीठ मुड़ी होगी तो वे आपको मेरे बारे में कई तरह की बातें बताएंगे। हो सकता है कि जब वे भगवान सुंदर चेहरों से बाहर निकले तो वे दरवाजे के पीछे नहीं थे, लेकिन स्वर्ग केवल जानता है कि वे कहाँ थे जब उन्होंने कृतज्ञता को विभाजित किया था।</t>
   </si>
   <si>
     <t>वे, वे</t>
   </si>
   <si>
-    <t>एमी, डैन और नेल्ली एक सम्मेलन कक्ष में एक मेज पर बैठे थे, फ्रेंकलिन दस्तावेजों के प्रजनन की जांच कर रहे थे-कुछ दुर्लभ, लाइब्रेरियन ने उसे बताया, केवल प्रतियां पेरिस में मौजूद थीं। "हाँ, यहाँ एक दुर्लभ किराने की सूची है," दान ने म्यूट कर दिया। "क्या बात है।</t>
+    <t>एमी, डैन और नेल्ली एक सम्मेलन कक्ष में एक मेज पर बैठे थे, फ्रैंकलिन दस्तावेजों के प्रजनन की जांच कर रहे थे-कुछ दुर्लभ, लाइब्रेरियन ने उसे बताया, केवल प्रतियां पेरिस में मौजूद थीं। "हाँ, यहाँ एक दुर्लभ किराने की सूची है," दान ने मौन कर दिया। "क्या बात है।</t>
   </si>
   <si>
     <t>लाइब्रेरियनग्रोसरी लिस्ट, फ्रैंकलिन डॉक्युमेंट्स के रिप्रोडक्शन, डॉक्यूमेंट्स</t>
@@ -434,37 +434,37 @@
     <t>मुझे, सुंदर किसान लड़कियां, किसान, किसान लड़कियां</t>
   </si>
   <si>
-    <t>द डेथ मिस्ट मदद के लिए नहीं है! "अखिल चिल्लाया।" यह दुख में नश्वर चिल्लाता है क्योंकि उनकी आत्मा अंडरवर्ल्ड में गुजरती है। यह निराशा की, मृत्यु की, टार्टरस की बहुत साँस है! "" बहुत बढ़िया, "पर्सी ने कहा।" क्या हम जाने के लिए दो आदेश प्राप्त कर सकते हैं?</t>
+    <t>द डेथ मिस्ट मदद करने के लिए नहीं है! "अखिल चिल्लाया।" यह दुख में नश्वर चिल्लाता है क्योंकि उनकी आत्मा अंडरवर्ल्ड में गुजरती है। यह निराशा की, मृत्यु का, टार्टरस का बहुत साँस है!</t>
   </si>
   <si>
     <t>अखिल</t>
   </si>
   <si>
-    <t>उसने मुझे सभ्यता समझाई। मेरा मतलब है कि यह उसे कैसा दिखता है। वह इसे थोड़ी देर और चलने देंगे। लेकिन यह बेहतर है कि सावधान रहें और अपने निजी जीवन में हस्तक्षेप न करें। यदि ऐसा होता है, तो वह भगवान को फोन करने और आदेश को रद्द करने के लिए उपयुक्त नहीं है।</t>
+    <t>उसने मुझे सभ्यता समझाई। मेरा मतलब है कि यह उसे कैसा दिखता है। वह इसे थोड़ी देर और चलने देगा। लेकिन यह बेहतर है कि सावधान रहें और अपने निजी जीवन में हस्तक्षेप न करें। यदि ऐसा होता है, तो वह भगवान को फोन करने और आदेश को रद्द करने के लिए उपयुक्त नहीं है।</t>
   </si>
   <si>
     <t>वह, वह, वह, वह, वह, उसका, उसका निजी जीवन</t>
   </si>
   <si>
-    <t>हम सचमुच यीशु के दिल में हैं, "उन्होंने कहा। मुझे लगा कि हम एक चर्च के तहखाने में हैं, लेकिन हम सचमुच यीशु के दिल में हैं।" खतरनाक हो, अपने दिल में कैंसर के साथ बच्चों को संग्रहीत।</t>
+    <t>हम सचमुच यीशु के दिल में हैं, "उन्होंने कहा। मुझे लगा कि हम एक चर्च के तहखाने में हैं, लेकिन हम सचमुच यीशु के दिल में हैं।" खतरनाक हो, अपने दिल में कैंसर के साथ बच्चों का भंडारण।</t>
   </si>
   <si>
     <t>उसने</t>
   </si>
   <si>
-    <t>क्या मैं पूछ सकता हूं कि आप कौन हैं, साहब? "" हाँ, मुझे उम्मीद है, "स्ट्राइक ने कहा, उसके पीछे चलना और दरवाजे की घंटी बजाना। एनिस्टिस के रात के खाने के निमंत्रण के बावजूद, वह अभी पुलिस के लिए सहानुभूति महसूस नहीं कर रहा था।" अपनी क्षमताओं के भीतर।</t>
+    <t>क्या मैं पूछ सकता हूं कि आप कौन हैं, साहब? "" हाँ, मैं ऐसी उम्मीद करता हूं, "स्ट्राइक ने कहा, उसके पीछे चलना और दरवाजे की घंटी बजाना। एनिस्टिस के रात के खाने के निमंत्रण के बावजूद, वह अभी पुलिस के लिए सहानुभूति महसूस नहीं कर रहा था।" अपनी क्षमताओं के भीतर।</t>
   </si>
   <si>
     <t>मैं, वह, पुलिस, आपका</t>
   </si>
   <si>
-    <t>मैंने जल्दी से पीछे हटने की कोशिश की लेकिन जेम्स ने मेरा हाथ पकड़ लिया। "चलो," उन्होंने कहा "यह मजेदार होगा।" Geez ... मज़ा की आपकी परिभाषा क्या है? कुज खानों ने संभवतः मेरे पहले दिन को यहां नहीं मारा। या शायद यह सिर्फ एक व्यक्तिगत लक्ष्य है, लेकिन फिर भी ...</t>
+    <t>मैंने जल्दी से पीछे हटने की कोशिश की लेकिन जेम्स ने मेरा हाथ पकड़ लिया। "चलो," उसने कहा "यह मजेदार होगा।" Geez ... मज़ा की आपकी परिभाषा क्या है? कुज खानों ने संभवतः मेरा पहला दिन यहां नहीं मारा। या शायद यह सिर्फ एक व्यक्तिगत लक्ष्य है, लेकिन फिर भी ...</t>
   </si>
   <si>
     <t>तुम्हारा, जेम्स, वह</t>
   </si>
   <si>
-    <t>ठीक है, फिर ठीक है। "उसने अपनी आँखें सिकोड़ ली।" आपके बारे में कैसे? क्या आपके पास कोई है ... रोमांस मुझे पता होना चाहिए? "" नहीं। एक नहीं। "" अच्छा, अच्छा। अति उत्कृष्ट। जब आप कॉलेज छोड़ कर नन बन जाएँगी तो लड़कों के लिए बहुत समय होगा। "वह मुस्कुराई।" मुझे खुशी है कि आपके लिए मेरे लिए ऐसे महत्वाकांक्षी सपने हैं।</t>
+    <t>ठीक है, ठीक है। "उसने अपनी आँखें सिकोड़ ली।" आपके बारे में कैसे? क्या आपके पास कोई है ... रोमांस मुझे पता होना चाहिए? "" नहींं। एक नहीं। "" अच्छा, अच्छा। अति उत्कृष्ट। जब आप कॉलेज छोड़ कर नन बन जाएँगी तो लड़कों के लिए बहुत समय होगा। "वह मुस्कुराई।" मुझे खुशी है कि आपके लिए मेरे लिए ऐसे महत्वाकांक्षी सपने हैं।</t>
   </si>
   <si>
     <t>वह, तुम, मैं, नन बन जाती हूं</t>
@@ -473,28 +473,28 @@
     <t>मेरी आंख के कोने से, मैं फेलिसिटी और एन को अपने गहनों पर टिका हुआ देख सकता हूं जैसे कि वे एक पुरातात्विक खुदाई से आकर्षक अवशेष थे। मैं ध्यान देता हूं कि उनके कंधे कांप रहे हैं, और मुझे एहसास है कि वे मेरी भयानक दुर्दशा पर हंसी लड़ रहे हैं। तुम्हारे लिए दोस्ती है।</t>
   </si>
   <si>
-    <t>फेलिसिटी, एन, उनके गहने, उनके, वे, दोस्ती</t>
-  </si>
-  <si>
-    <t>गैन्किस ने एक हाथ उठाकर दूर की चट्टान की ओर इशारा किया। "और इसके चेहरे में हजारों छोटे छेद थे, थोड़ा क्या-क्या-आप-कॉल ... '" अल्कॉव्स, "केनीत ने लगभग स्वप्निल स्वर में आपूर्ति की। "मैं उन्हें अल्कोव्स, गैंकिस कहता हूं। जैसा कि आप अपनी मातृभाषा में बोल सकते हैं।</t>
+    <t>फेलिसिटी, ऐन, उनके गहने, उनके, वे, दोस्ती</t>
+  </si>
+  <si>
+    <t>गैन्किस ने एक हाथ उठाकर दूर की चट्टान की ओर इशारा किया। "और उसके चेहरे में हजारों छोटे छेद थे, थोड़ा क्या आप-कॉल-'...'" अल्कॉव्स, "केनीत ने लगभग एक स्वप्निल स्वर में आपूर्ति की। "मैं उन्हें अल्कोव्स, गैंकिस कहता हूं। जैसा कि आप अपनी मातृभाषा में बोल सकते हैं।</t>
   </si>
   <si>
     <t>Gankis, आप</t>
   </si>
   <si>
-    <t>यह बहुत अच्छा है, "केटी ने कहा।" वास्तव में, यह क्रांतिकारी है। यदि आप काम कर सकते हैं और एक ही समय में प्यार कर सकते हैं, तो आप पहली महिला हैं जो मुझे कभी पता था कि वह कर सकती थी। हो सकता है कि आप मिसिंग लिंक हों, अमांडा। "हो सकता है कि आपको 'लेडीज होम जर्नल' के लिए नौकरी मिल जाए। उन्हें सादगी पसंद है।</t>
+    <t>यह बहुत अच्छा है, "केटी ने कहा।" वास्तव में, यह क्रांतिकारी है। यदि आप एक ही समय में काम कर सकते हैं और प्यार में हो सकते हैं, तो आप पहली महिला हैं जो मुझे कभी पता चला था। हो सकता है कि आप मिसिंग लिंक हों, अमांडा। "हो सकता है कि आपको 'लेडीज होम जर्नल' के लिए नौकरी मिल जाए। उन्हें सादगी पसंद शिट पसंद है।</t>
   </si>
   <si>
     <t>आप, अमांडा, आप, लेडीज होम जर्नल, वे</t>
   </si>
   <si>
-    <t>डॉक्टर विशेष रूप से इस तथ्य से परेशान लग रहे थे कि डकैती अप्रत्याशित थी, और रात के समय में प्रयास किया गया था; जैसे कि यह दोपहर में व्यापार करने के लिए हाउसब्रीकिंग तरीके से सज्जनों की स्थापना की प्रथा थी, और एक या दो दिन पहले, ट्वोपनी पोस्ट द्वारा एक नियुक्ति करने के लिए।</t>
+    <t>डॉक्टर विशेष रूप से इस तथ्य से परेशान लग रहे थे कि डकैती अप्रत्याशित थी, और रात के समय में प्रयास किया गया था; जैसे कि यह दोपहर में कारोबार करने के लिए हाउसब्रीकिंग तरीके से सज्जनों की स्थापना की गई थी, और एक या दो दिन पहले, ट्वोपनी पोस्ट द्वारा एक नियुक्ति करने के लिए।</t>
   </si>
   <si>
     <t>चिकित्सक</t>
   </si>
   <si>
-    <t>वह उससे पूछती थी कि उसमें ऐसा क्या है, जो कुछ भी नहीं कर रहा है, लेकिन फिर किसी को देखने के लिए बोलने के लिए जाग रहा है। उन्होंने कहा कि यह गहरी और संतोषजनक नींद से जागने जैसा था, जब आप अपनी आँखें बंद रखते हैं तो सवाल पूछे जाते हैं। वह काफी खुश था। वैसे भी दृष्टि को ओवर-रेटेड किया गया था।</t>
+    <t>वह उससे पूछती थी कि उसमें ऐसा क्या है, जो कुछ भी नहीं कर रहा है, लेकिन फिर किसी को देखने के लिए बोलने के लिए जाग रहा है। उन्होंने कहा कि यह गहरी और संतोषजनक नींद से जागने जैसा था, जब आप अपनी आँखें बंद रखते हैं तो सवाल पूछे जाते हैं। वह काफी खुश था। वैसे भी दृष्टि को ओवर रेटिंग दी गई थी।</t>
   </si>
   <si>
     <t>वह चाहती थी</t>
@@ -512,106 +512,106 @@
     <t>चाची और चाचा, आप, उनकी चाची और चाचा</t>
   </si>
   <si>
-    <t>तैयार हो? ”जयम ने गूँज कर कहा।“ हाँ, हाँ, मैं तैयार हूँ। मैं बहुत सारे तरल पदार्थ पीने के लिए तैयार हूं और पूरे दिन बेहोश होकर सोफे पर पड़ा रहता हूं। यही मैं तैयार हूं। मैं किसी भी प्रकार की शारीरिक गतिविधि में संलग्न नहीं हो सकता या मेरा सिर एकदम से गिर जाएगा। क्या आप निक चाहते हैं? क्योंकि अगर ऐसा है, तो मुझे वह चोट लगी है।</t>
+    <t>तैयार? "जयम ने गूँज कर कहा।" हाँ, हाँ, मैं तैयार हूँ। मैं बहुत सारे तरल पदार्थ पीने के लिए तैयार हूं और पूरे दिन बेहोश होकर सोफे पर पड़ा रहता हूं। यही मैं तैयार हूं। मैं किसी भी प्रकार की शारीरिक गतिविधि में संलग्न नहीं हो सकता या मेरा सिर एकदम से गिर जाएगा। क्या आप निक चाहते हैं? क्योंकि अगर ऐसा है, तो मुझे लगता है कि चोट लगी है।</t>
   </si>
   <si>
     <t>छेद</t>
   </si>
   <si>
-    <t>हत्या करने वाले चोर यहाँ अपना घर बनाते हैं। "वह उसकी आवाज़ से कंपकंपी को रोकने में नाकाम रही।" बिल्कुल, "अनस ने जवाब दिया।" खतरनाक जानवर भी। "" बिना किसी शक के। "उसने उसकी ओर एक नज़र देखा।" "उन्होंने एक खर्राटे का दमन किया।" ओह, ऐसी तारीफ, आपका उच्चाटन। तुम मुझे ब्लश करने जा रहे हो।</t>
+    <t>हत्या करने वाले चोर यहाँ अपना घर बनाते हैं। "वह उसकी आवाज़ से कंपकंपी को रोकने में नाकाम रही।" बिल्कुल, "अनस ने जवाब दिया।" खतरनाक जानवर भी। "" बिना किसी शक के। "उसने उसकी ओर एक नज़र देखा।" "उसने एक खर्राटे का दमन किया।" ओह, ऐसी तारीफ, आपका उच्चाटन। तुम मुझे ब्लश करने जा रहे हो।</t>
   </si>
   <si>
     <t>जोनास, वह</t>
   </si>
   <si>
-    <t>श्री बेनेट, आप इस तरह से अपने बच्चों का दुरुपयोग कैसे कर सकते हैं? आप मुझे खुश करने में आनंद लें। आपको मेरी गरीब नसों पर कोई दया नहीं है। "" तुम मुझसे गलती करते हो, मेरे प्यारे। आपकी नसों के प्रति मेरा बहुत सम्मान है। वे मेरे पुराने दोस्त हैं। मैंने सुना है कि आपने पिछले बीस वर्षों में कम से कम इनका उल्लेख किया है।</t>
-  </si>
-  <si>
-    <t>जब रोज़ चीखने लगती है, तो वह ज़ोर से शुरू होती है, ज़ोर से चलती है, और ज़ोर से खत्म होती है। गुलाब के कान बहुत अच्छे हैं और हमेशा एक ही नोट पर चिल्लाता है। इससे पहले कि मैं पुस्तकालय और उसके साथ हमारे पियानो को जलाता, मैंने उसका परीक्षण किया। नोट बी फ्लैट पर गुलाब चिल्लाता है। हमें अब एक पियानो की आवश्यकता नहीं है कि हमारे पास एक मानव ट्यूनिंग कांटा है।</t>
+    <t>श्री बेनेट, आप इस तरह से अपने बच्चों का दुरुपयोग कैसे कर सकते हैं? तुम मुझे खुश करने में लग जाओ। आपको मेरी गरीब नसों पर कोई दया नहीं है। "" तुम मुझसे गलती करते हो, मेरे प्यारे। आपकी नसों के प्रति मेरा बहुत सम्मान है। वे मेरे पुराने दोस्त हैं। मैंने सुना है कि आप कम से कम इन पिछले बीस वर्षों में उनका उल्लेख करते हैं।</t>
+  </si>
+  <si>
+    <t>जब रोज़ चीखने लगती है, तो वह ज़ोर से शुरू होती है, ज़ोर से चलती है, और ज़ोर से खत्म होती है। गुलाब का कान बहुत अच्छा है और हमेशा एक ही नोट पर चिल्लाता है। इससे पहले कि मैं पुस्तकालय जलाता, उसके साथ हमारे पियानो और उसके साथ मैं उसका परीक्षण कर लेता। नोट बी फ्लैट पर गुलाब चिल्लाता है। हमें अब एक पियानो की आवश्यकता नहीं है कि हमारे पास एक मानव ट्यूनिंग कांटा है।</t>
   </si>
   <si>
     <t>गुलाब का फूल</t>
   </si>
   <si>
-    <t>... भले ही मैं टोयाह में किसी भी बच्चे की तुलना में घर पर बेहतर शिक्षा प्राप्त कर रहा था, मुझे तेरह साल की उम्र में, जब मैं तेरह साल का था, सामाजिक अनुदान प्राप्त करने और डिप्लोमा हासिल करने के लिए स्कूल जाने की आवश्यकता थी। क्योंकि इस दुनिया में, पिताजी ने कहा, यह एक अच्छी शिक्षा के लिए पर्याप्त नहीं है। आपको इसे साबित करने के लिए आपको एक कागज़ का टुकड़ा चाहिए।</t>
+    <t>... भले ही मैं टोयाह में किसी भी बच्चे की तुलना में घर पर बेहतर शिक्षा प्राप्त कर रहा था, मुझे तेरह साल की उम्र में, जब मैं तेरह वर्ष का था, सामाजिक अनुदान प्राप्त करने और डिप्लोमा हासिल करने के लिए स्कूल जाने की आवश्यकता थी। क्योंकि इस दुनिया में, पिताजी ने कहा, यह एक अच्छी शिक्षा के लिए पर्याप्त नहीं है। आपको इसे साबित करने के लिए कागज के टुकड़े की आवश्यकता है।</t>
   </si>
   <si>
     <t>विश्व</t>
   </si>
   <si>
-    <t>क्या? आप किससे शादी कर रहे हैं? "उसका जबड़ा कड़ा हो गया।" राजकुमारी क्लियोना बेलोस। "लूसिया उसके कानों पर विश्वास नहीं कर सकती थी।" यह व्यवस्था की गई है। "मैग्नस ने उसे एक नज़र दिया।" ओह, बिल्कुल नहीं। अपने पिता के राज्य को लेने और उसके जीवन को नष्ट करने में मदद करने के बाद से, मैं मदद नहीं कर सका लेकिन उसके साथ प्यार में पागल हो गया। हां, जाहिर है कि इसकी व्यवस्था की गई थी।</t>
+    <t>क्या? आप किससे शादी कर रहे हैं? "उसका जबड़ा कड़ा हो गया।" राजकुमारी क्लियोना बेलोस। "लूसिया को उसके कानों पर विश्वास नहीं हो रहा था।" यह व्यवस्था की गई है। "मैग्नस ने उसे एक नज़र दिया।" ओह, बिल्कुल नहीं। अपने पिता के राज्य को लेने और उसके जीवन को नष्ट करने में मदद करने के बाद से, मैं मदद नहीं कर सका लेकिन उसके साथ प्यार में पागल हो गया। हां, जाहिर है कि इसकी व्यवस्था की गई थी।</t>
   </si>
   <si>
     <t>लुसिया</t>
   </si>
   <si>
-    <t>और आपकी रुचियां और शौक क्या हैं, निकोलस? "एनाबेल ने बेहिचक पूछा, एक टेलीविजन साक्षात्कारकर्ता और एक बंधक के बीच एक क्रॉस की तरह लग रहा था। निक ने एक मिनट के लिए इस पर विचार किया, और फिर कहा" मुझे तलवार पसंद है। "एनाबेल ने अपनी प्लेट पर झुक कर पूछा। उसकी आवाज़ बदल रही है "तुम बाड़?"</t>
+    <t>और आपकी रुचियां और शौक क्या हैं, निकोलस? "एनाबेल ने बेहिचक पूछा, एक टेलीविजन साक्षात्कारकर्ता और एक बंधक के बीच एक क्रॉस की तरह लग रहा था। निक ने एक मिनट के लिए इस पर विचार किया, और फिर कहा" मुझे तलवार पसंद है। "एनाबेल ने अपनी प्लेट पर झुक कर पूछा। , उसकी आवाज़ बदल रही है "तुम बाड़?"</t>
   </si>
   <si>
     <t>एनाबेल</t>
   </si>
   <si>
-    <t>आपने इस घर में आधी किताबें पढ़ी हैं? यह पूरा घर? "" ठीक है, लगभग आधा। "स्टिकी ने कहा।" अधिक सटीक होने के लिए, मुझे लगता है कि मैंने और अधिक पढ़ा है "- उसकी आँखें गणना करते हुए ऊपर चली गईं -" तीन सातवें? हाँ, तीन सातवें। "" केवल तीन सातवें? "केट ने निराश दिखने का नाटक करते हुए कहा।" और यहाँ मैं प्रभावित होने के लिए तैयार था।</t>
+    <t>आपने इस घर में आधी किताबें पढ़ी हैं? यह पूरा घर? "" ठीक है, लगभग आधा। "स्टिकी ने कहा।" अधिक सटीक होने के लिए, मुझे लगता है कि मैंने और अधिक पढ़ा है "- उसकी आँखों की गणना के रूप में उसकी आँखें ऊपर चली गईं -" तीन सातवें? हाँ, तीन सातवें। "" केवल तीन सातवें? "केट ने निराश दिखने का नाटक करते हुए कहा।" और यहाँ मैं प्रभावित होने के लिए तैयार थी।</t>
   </si>
   <si>
     <t>चिपचिपा</t>
   </si>
   <si>
-    <t>अगर मुझे परवाह नहीं है तो भी क्या होगा? वू-हू, इतना डरावना। ओह, कृपया, कृपया, मुझे जामुन से बचाओ! "राक्षस ने उसे चौकस देखा। कितना अजीब है, यह कहा। आपके द्वारा कहे गए शब्द मुझे बताते हैं कि आप जामुन से डरते हैं, लेकिन आपके कार्यों से अन्यथा लगता है।</t>
+    <t>अगर मुझे परवाह नहीं है तो भी क्या होगा? वू-हू, इतना डरावना। ओह, कृपया, कृपया, मुझे जामुन से बचाओ! "राक्षस ने उसे चतुराई से देखा। कितना अजीब है, यह कहा। मेरे द्वारा कहे गए शब्द आपको बताते हैं कि आप जामुन से डरते हैं, लेकिन आपके कार्यों से अन्यथा लगता है।</t>
   </si>
   <si>
     <t>राक्षस</t>
   </si>
   <si>
-    <t>मुझे यकीन है कि मुझे कोई अंदाजा नहीं है कि आप PRINCESS के बारे में क्या बात कर रहे हैं। "जब उसने आखिरी शब्द कहा, तो उसने अपना सिर झुका लिया और आधा रूखा हो गया।" यही है जिसके बारे में मैं बात कर रहा हूँ। चूंकि हम दूसरों में भाग गए हैं, आप सामान्य से अधिक ठंडे और घमंडी रहे हैं। "उसने अपनी आवाज कम रखी ताकि दूसरों को सुनाई न दे।" क्या ऐसा है? मैं कहूंगा कि मैं घमंडी था</t>
-  </si>
-  <si>
-    <t>ठीक है, हम इस जगह से कैसे बाहर निकलते हैं? "आइवाइट की आवाज़ थोड़ी हिलती हुई है।" हम नहीं कर सकते। "अगर कालेब को लगता है कि उसे कोई निराशा नहीं है, तो वह उसे बता नहीं रहा था। उसने बड़े इत्मीनान से देखा," जब तक हम किसी को हमारी मदद करने के लिए तैयार नहीं पाते। "" ठीक है, कि एक समस्या नहीं होनी चाहिए, "ट्रिस्टन ने अपने हाथों को फेंकते हुए कहा," अब तक की हर चीज को देखते हुए हमें मारने की कोशिश की गई है!</t>
+    <t>मुझे यकीन है कि मुझे पता नहीं है कि आप PRINCESS के बारे में क्या बात कर रहे हैं। "जब उसने आखिरी शब्द कहा तो उसने अपना सिर झुका लिया और आधा रूखा हो गया।" यही है जिसके बारे में मैं बात कर रहा हूँ। चूंकि हम दूसरों में भाग गए हैं आप सामान्य से अधिक ठंडे और घमंडी रहे हैं। "उसने अपनी आवाज कम रखी ताकि दूसरों को सुनाई न दे।" क्या ऐसा है? मैं कहूंगा कि मैं घमंडी था</t>
+  </si>
+  <si>
+    <t>खैर, हम इस जगह से कैसे बाहर निकलते हैं? "आइवाइट की आवाज़ थोड़ी हिलती हुई है।" हम नहीं कर सकते। "अगर कालेब को लगा कि उसे कोई निराशा नहीं है, तो वह उसे समझा नहीं रहा था। उसने बड़े इत्मीनान से देखा," जब तक हम किसी को हमारी मदद करने के लिए तैयार नहीं पाते। "" ठीक है, कि एक समस्या नहीं होनी चाहिए, "ट्रिस्टन ने अपने हाथों को फेंकते हुए कहा," अब तक की हर चीज को देखते हुए हमें मारने की कोशिश की गई है!</t>
   </si>
   <si>
     <t>कालेब</t>
   </si>
   <si>
-    <t>मैं इसके लिए सहायता के लिए इयान को न्यू ऑरलियन्स में स्थानांतरित कर रहा हूं, "आर्क ने कहा, जैसा कि उसने दोनों पुरुषों को देखा।" वे अभी भी हनीमून चरण में हैं। "उन्होंने अपनी उंगलियों के साथ एक उद्धरण प्रस्ताव बनाया। पीटर और विन्सेन्ट ने भयभीत रूप का आदान-प्रदान किया, इससे पहले कि पीटर ने जवाब दिया।" कृपया, हमें उस यातना के माध्यम से मत डालें।</t>
-  </si>
-  <si>
-    <t>शाइनी, अन्ना</t>
-  </si>
-  <si>
-    <t>वह पागल है, "ब्रूनो ने कहा, उसके सिर के चारों ओर हलकों में एक उंगली घुमाते हुए और यह संकेत देने के लिए कि वह कितना पागल था, यह बताने के लिए सीटी बजाता है।" वह दूसरे दिन सड़क पर एक बिल्ली के पास गया और उसे दोपहर की चाय के लिए आमंत्रित किया। । "" बिल्ली ने क्या कहा? "ग्रेटेल से पूछा, जो रसोई के कोने में एक सैंडविच बना रहा था।" कुछ नहीं। "ब्रूनो ने समझाया।" यह एक बिल्ली थी।</t>
+    <t>मैं इसके लिए सहायता करने के लिए इयान को न्यू ऑरलियन्स में स्थानांतरित कर रहा हूं, "आर्क ने कहा कि वह दोनों पुरुषों को देखता था।" वे अभी भी हनीमून चरण में हैं। "उन्होंने अपनी उंगलियों के साथ एक उद्धरण प्रस्ताव बनाया। पीटर ने जवाब देने से पहले पीटर और विंसेंट ने भयावह रूप का आदान-प्रदान किया।" कृपया, हमें उस यातना के माध्यम से न डालें।</t>
+  </si>
+  <si>
+    <t>Shayne, Anna</t>
+  </si>
+  <si>
+    <t>He's crazy," Bruno said, twirling a finger in circles around the side of his head and whistling to indicate just how crazy he thought he was. "He went up to a cat on the street the other day and invited her over for afternoon tea." "What did the cat say?" asked Gretel, who was making a sandwich in the corner of the kitchen. "Nothing." explained Bruno. "It was a cat.</t>
   </si>
   <si>
     <t>ग्रेटेल</t>
   </si>
   <si>
-    <t>आपका अब तक का पहला हफ्ता कैसा है? "इसाबेल पूछती है।" ठीक है, मुझे देखने दो, "मैं शुरू करता हूं।" क्लो कहती है कि मेरी कलम चमक रही है, और मैं आज सुबह केवल तीस मिनट का था, जिसका स्पष्ट अर्थ है कि मुझे देर हो रही है, लेकिन उज्ज्वल पक्ष, वह सोचती है कि उसका गैर-वसा, आधा मीठा, नो-व्हिप सोया लट्टे का स्वाद सही नहीं था और फिर उसने मुझे बताया कि वह इसके लिए भुगतान नहीं कर रही है। इसके अलावा, काम ठीक है।</t>
-  </si>
-  <si>
-    <t>work</t>
-  </si>
-  <si>
-    <t>आइजनहावर और पैटन, पुराने मित्रों और मित्र राष्ट्रों की आगामी सफलता के लिए महत्वपूर्ण आंकड़े, पैटन के हिस्से पर अभी तक एक और गफ से सम्मानित किया गया जो उसे उसकी कमान का खर्च दे सकता था। पैटन का सिर कृतज्ञता में इके के कंधे पर है, लेकिन सीन को आइजनहावर के आंतरिक सवाल से पूरी तरह से मुद्लिन होने से बचाया गया है कि क्या पैटन बिस्तर पर अपने वर्तमान हेलमेट पहनता है।</t>
-  </si>
-  <si>
-    <t>Patton</t>
-  </si>
-  <si>
-    <t>उसने अपने गले के पीछे घृणा की आवाज की। "ओह, आपका बहुत-बहुत धन्यवाद। यही हर आदमी अपने नाम के बारे में सुनना चाहता है। आप मुझे 'लिटिल पीकर' भी कह सकते हैं, जबकि आप मुझे बता रहे हैं कि आप मुझे स्त्री स्वच्छता के लिए आपके साथ खरीदारी करना पसंद करेंगे। उत्पादों। ओह और हर तरह से, उस पर फूलों के साथ एक बड़ा, स्पार्कलिंग गुलाबी बैग ले और मुझे इसे पकड़ो।</t>
+    <t>आपका अब तक का पहला हफ्ता कैसा है? "इसाबेल पूछती है।" ठीक है, मुझे देखने दो, "मैं शुरू करता हूं।" क्लो कहता है कि मेरी कलम की चमक खराब है, और मैं आज सुबह केवल तीस मिनट का था, जिसका स्पष्ट अर्थ है कि मुझे देर हो रही है, लेकिन उज्ज्वल पक्ष, वह सोचती है कि उसका गैर-वसा, आधा मीठा, नो-व्हिप सोया लट्टे का स्वाद सही नहीं था और फिर उसने मुझे बताया कि वह इसके लिए भुगतान नहीं कर रही है। इसके अलावा, काम सिर्फ ठीक है।</t>
+  </si>
+  <si>
+    <t>काम क</t>
+  </si>
+  <si>
+    <t>आइजनहावर और पैटन, पुराने मित्रों और मित्र राष्ट्रों की आगामी सफलता के लिए महत्वपूर्ण आंकड़े, पैटन के हिस्से पर अभी तक एक और गफ से सम्मानित किया गया जो उसे उसकी कमान का खर्च दे सकता था। पैटन का सिर आभार में इके के कंधे पर है, लेकिन सीन को आइज़ेनहॉवर के आंतरिक प्रश्न से पूरी तरह से उथल-पुथल से बचाया जाता है कि क्या पैटन बिस्तर पर अपने वर्तमान हेलमेट पहनता है।</t>
+  </si>
+  <si>
+    <t>पैटन</t>
+  </si>
+  <si>
+    <t>उसने अपने गले के पीछे घृणा की आवाज की। "ओह, आपका बहुत-बहुत धन्यवाद। यही कि हर आदमी अपने नाम के बारे में सुनना चाहता है। आप मुझे 'लिटिल पीकर' भी कह सकते हैं, जबकि आप मुझे बता रहे हैं कि आप मुझे स्त्री स्वच्छता के लिए आपके साथ खरीदारी करना पसंद करेंगे। उत्पादों। ओह और हर तरह से, उस पर फूलों के साथ एक बड़ा, स्पार्कलिंग गुलाबी बैग ले लो और मुझे इसे पकड़ो।</t>
   </si>
   <si>
     <t>you</t>
   </si>
   <si>
-    <t>Owr brave little shank!</t>
-  </si>
-  <si>
-    <t>shank</t>
+    <t>उल्लू बहादुर थोड़ा टांग!</t>
+  </si>
+  <si>
+    <t>टांग</t>
   </si>
   <si>
     <t>Go make love to a tube sock.</t>
   </si>
   <si>
-    <t>ट्यूब जुर्राब, बाहर</t>
+    <t>tube sock, Outside</t>
   </si>
   <si>
     <t>A woman's weapon is her tongue.</t>

</xml_diff>